<commit_message>
Fix hiển thị ngày thêm số 0 truwowscc những ngày và tháng nhỏ hơn 10
Fix hiển thị ngày thêm số 0 truwowscc những ngày và tháng nhỏ hơn 10
</commit_message>
<xml_diff>
--- a/src/views/FileMauExportDanhMuc/DanToc.xlsx
+++ b/src/views/FileMauExportDanhMuc/DanToc.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>STT</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>Ten</t>
+  </si>
+  <si>
+    <t>Chăm</t>
   </si>
 </sst>
 </file>
@@ -113,12 +116,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -460,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,6 +566,14 @@
         <v>11</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>

</xml_diff>